<commit_message>
add check for products categories
</commit_message>
<xml_diff>
--- a/MMAPlus_Merchandising/MMAPlus_Merchandising.xlsx
+++ b/MMAPlus_Merchandising/MMAPlus_Merchandising.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Distribution Point" sheetId="11" r:id="rId1"/>
@@ -1228,7 +1228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1363,18 +1363,13 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1760,7 +1755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T973"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1840,16 +1835,16 @@
       <c r="P1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="139" t="s">
+      <c r="Q1" s="133" t="s">
         <v>203</v>
       </c>
-      <c r="R1" s="139" t="s">
+      <c r="R1" s="133" t="s">
         <v>204</v>
       </c>
-      <c r="S1" s="139" t="s">
+      <c r="S1" s="133" t="s">
         <v>205</v>
       </c>
-      <c r="T1" s="139" t="s">
+      <c r="T1" s="133" t="s">
         <v>206</v>
       </c>
     </row>
@@ -44296,9 +44291,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J158"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44694,18 +44689,18 @@
       <c r="A14" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B14" s="131" t="s">
+      <c r="B14" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="131" t="s">
+      <c r="C14" s="134" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="132"/>
-      <c r="E14" s="132"/>
-      <c r="F14" s="132"/>
-      <c r="G14" s="132"/>
-      <c r="H14" s="132"/>
-      <c r="I14" s="132"/>
+      <c r="D14" s="134"/>
+      <c r="E14" s="134"/>
+      <c r="F14" s="134"/>
+      <c r="G14" s="134"/>
+      <c r="H14" s="134"/>
+      <c r="I14" s="134"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -44745,28 +44740,28 @@
       <c r="A17" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="134" t="s">
+      <c r="B17" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="134" t="s">
+      <c r="C17" s="130" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="134">
+      <c r="D17" s="130">
         <v>1</v>
       </c>
-      <c r="E17" s="134">
+      <c r="E17" s="130">
         <v>2</v>
       </c>
-      <c r="F17" s="134">
+      <c r="F17" s="130">
         <v>3</v>
       </c>
-      <c r="G17" s="134">
+      <c r="G17" s="130">
         <v>1</v>
       </c>
-      <c r="H17" s="134">
+      <c r="H17" s="130">
         <v>2</v>
       </c>
-      <c r="I17" s="134">
+      <c r="I17" s="130">
         <v>3</v>
       </c>
     </row>
@@ -44774,28 +44769,28 @@
       <c r="A18" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B18" s="134" t="s">
+      <c r="B18" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="134" t="s">
+      <c r="C18" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="134">
+      <c r="D18" s="130">
         <v>1</v>
       </c>
-      <c r="E18" s="134">
+      <c r="E18" s="130">
         <v>10</v>
       </c>
-      <c r="F18" s="134">
+      <c r="F18" s="130">
         <v>21</v>
       </c>
-      <c r="G18" s="134">
+      <c r="G18" s="130">
         <v>1</v>
       </c>
-      <c r="H18" s="134">
+      <c r="H18" s="130">
         <v>10</v>
       </c>
-      <c r="I18" s="134">
+      <c r="I18" s="130">
         <v>21</v>
       </c>
     </row>
@@ -44803,28 +44798,28 @@
       <c r="A19" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B19" s="134" t="s">
+      <c r="B19" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="134" t="s">
+      <c r="C19" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="134">
+      <c r="D19" s="130">
         <v>2</v>
       </c>
-      <c r="E19" s="134">
+      <c r="E19" s="130">
         <v>11</v>
       </c>
-      <c r="F19" s="134">
+      <c r="F19" s="130">
         <v>22</v>
       </c>
-      <c r="G19" s="134">
+      <c r="G19" s="130">
         <v>2</v>
       </c>
-      <c r="H19" s="134">
+      <c r="H19" s="130">
         <v>11</v>
       </c>
-      <c r="I19" s="134">
+      <c r="I19" s="130">
         <v>22</v>
       </c>
     </row>
@@ -45265,8 +45260,8 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="135"/>
-      <c r="I35" s="135"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
@@ -45306,28 +45301,28 @@
       <c r="A38" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="B38" s="134" t="s">
+      <c r="B38" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="134" t="s">
+      <c r="C38" s="130" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="134">
+      <c r="D38" s="130">
         <v>1</v>
       </c>
-      <c r="E38" s="134">
+      <c r="E38" s="130">
         <v>2</v>
       </c>
-      <c r="F38" s="134">
+      <c r="F38" s="130">
         <v>3</v>
       </c>
-      <c r="G38" s="134">
+      <c r="G38" s="130">
         <v>1</v>
       </c>
-      <c r="H38" s="134">
+      <c r="H38" s="130">
         <v>2</v>
       </c>
-      <c r="I38" s="134">
+      <c r="I38" s="130">
         <v>3</v>
       </c>
     </row>
@@ -45335,28 +45330,28 @@
       <c r="A39" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="B39" s="134" t="s">
+      <c r="B39" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="134" t="s">
+      <c r="C39" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="134">
+      <c r="D39" s="130">
         <v>1</v>
       </c>
-      <c r="E39" s="134">
+      <c r="E39" s="130">
         <v>10</v>
       </c>
-      <c r="F39" s="134">
+      <c r="F39" s="130">
         <v>21</v>
       </c>
-      <c r="G39" s="134">
+      <c r="G39" s="130">
         <v>1</v>
       </c>
-      <c r="H39" s="134">
+      <c r="H39" s="130">
         <v>10</v>
       </c>
-      <c r="I39" s="134">
+      <c r="I39" s="130">
         <v>21</v>
       </c>
     </row>
@@ -45364,28 +45359,28 @@
       <c r="A40" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="B40" s="134" t="s">
+      <c r="B40" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="134" t="s">
+      <c r="C40" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="D40" s="134">
+      <c r="D40" s="130">
         <v>2</v>
       </c>
-      <c r="E40" s="134">
+      <c r="E40" s="130">
         <v>11</v>
       </c>
-      <c r="F40" s="134">
+      <c r="F40" s="130">
         <v>22</v>
       </c>
-      <c r="G40" s="134">
+      <c r="G40" s="130">
         <v>2</v>
       </c>
-      <c r="H40" s="134">
+      <c r="H40" s="130">
         <v>11</v>
       </c>
-      <c r="I40" s="134">
+      <c r="I40" s="130">
         <v>22</v>
       </c>
     </row>
@@ -45654,28 +45649,28 @@
       <c r="A50" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="B50" s="133" t="s">
+      <c r="B50" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="133" t="s">
+      <c r="C50" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D50" s="135">
+      <c r="D50" s="2">
         <v>3</v>
       </c>
-      <c r="E50" s="135">
+      <c r="E50" s="2">
         <v>13</v>
       </c>
-      <c r="F50" s="135">
+      <c r="F50" s="2">
         <v>23</v>
       </c>
-      <c r="G50" s="135">
+      <c r="G50" s="2">
         <v>3</v>
       </c>
-      <c r="H50" s="135">
+      <c r="H50" s="2">
         <v>13</v>
       </c>
-      <c r="I50" s="135">
+      <c r="I50" s="2">
         <v>23</v>
       </c>
     </row>
@@ -45741,28 +45736,28 @@
       <c r="A53" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B53" s="134" t="s">
+      <c r="B53" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C53" s="134" t="s">
+      <c r="C53" s="130" t="s">
         <v>57</v>
       </c>
-      <c r="D53" s="134">
+      <c r="D53" s="130">
         <v>1</v>
       </c>
-      <c r="E53" s="134">
+      <c r="E53" s="130">
         <v>2</v>
       </c>
-      <c r="F53" s="134">
+      <c r="F53" s="130">
         <v>3</v>
       </c>
-      <c r="G53" s="134">
+      <c r="G53" s="130">
         <v>1</v>
       </c>
-      <c r="H53" s="134">
+      <c r="H53" s="130">
         <v>2</v>
       </c>
-      <c r="I53" s="134">
+      <c r="I53" s="130">
         <v>3</v>
       </c>
     </row>
@@ -45770,28 +45765,28 @@
       <c r="A54" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B54" s="134" t="s">
+      <c r="B54" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C54" s="134" t="s">
+      <c r="C54" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="D54" s="134">
+      <c r="D54" s="130">
         <v>1</v>
       </c>
-      <c r="E54" s="134">
+      <c r="E54" s="130">
         <v>10</v>
       </c>
-      <c r="F54" s="134">
+      <c r="F54" s="130">
         <v>21</v>
       </c>
-      <c r="G54" s="134">
+      <c r="G54" s="130">
         <v>1</v>
       </c>
-      <c r="H54" s="134">
+      <c r="H54" s="130">
         <v>10</v>
       </c>
-      <c r="I54" s="134">
+      <c r="I54" s="130">
         <v>21</v>
       </c>
     </row>
@@ -45799,28 +45794,28 @@
       <c r="A55" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B55" s="134" t="s">
+      <c r="B55" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C55" s="134" t="s">
+      <c r="C55" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="D55" s="134">
+      <c r="D55" s="130">
         <v>2</v>
       </c>
-      <c r="E55" s="134">
+      <c r="E55" s="130">
         <v>11</v>
       </c>
-      <c r="F55" s="134">
+      <c r="F55" s="130">
         <v>22</v>
       </c>
-      <c r="G55" s="137">
+      <c r="G55" s="130">
         <v>2</v>
       </c>
-      <c r="H55" s="137">
+      <c r="H55" s="130">
         <v>11</v>
       </c>
-      <c r="I55" s="137">
+      <c r="I55" s="130">
         <v>22</v>
       </c>
     </row>
@@ -46272,19 +46267,19 @@
       <c r="D71" s="2">
         <v>4</v>
       </c>
-      <c r="E71" s="135">
+      <c r="E71" s="2">
         <v>14</v>
       </c>
-      <c r="F71" s="135">
+      <c r="F71" s="2">
         <v>24</v>
       </c>
-      <c r="G71" s="135">
+      <c r="G71" s="2">
         <v>4</v>
       </c>
-      <c r="H71" s="135">
+      <c r="H71" s="2">
         <v>14</v>
       </c>
-      <c r="I71" s="135">
+      <c r="I71" s="2">
         <v>24</v>
       </c>
     </row>
@@ -46352,28 +46347,28 @@
       <c r="A74" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="B74" s="134" t="s">
+      <c r="B74" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C74" s="134" t="s">
+      <c r="C74" s="130" t="s">
         <v>57</v>
       </c>
-      <c r="D74" s="134">
+      <c r="D74" s="130">
         <v>1</v>
       </c>
-      <c r="E74" s="134">
+      <c r="E74" s="130">
         <v>2</v>
       </c>
-      <c r="F74" s="134">
+      <c r="F74" s="130">
         <v>3</v>
       </c>
-      <c r="G74" s="134">
+      <c r="G74" s="130">
         <v>1</v>
       </c>
-      <c r="H74" s="134">
+      <c r="H74" s="130">
         <v>2</v>
       </c>
-      <c r="I74" s="134">
+      <c r="I74" s="130">
         <v>3</v>
       </c>
     </row>
@@ -46381,28 +46376,28 @@
       <c r="A75" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="B75" s="134" t="s">
+      <c r="B75" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C75" s="134" t="s">
+      <c r="C75" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="D75" s="134">
+      <c r="D75" s="130">
         <v>1</v>
       </c>
-      <c r="E75" s="134">
+      <c r="E75" s="130">
         <v>10</v>
       </c>
-      <c r="F75" s="134">
+      <c r="F75" s="130">
         <v>21</v>
       </c>
-      <c r="G75" s="134">
+      <c r="G75" s="130">
         <v>1</v>
       </c>
-      <c r="H75" s="134">
+      <c r="H75" s="130">
         <v>10</v>
       </c>
-      <c r="I75" s="134">
+      <c r="I75" s="130">
         <v>21</v>
       </c>
     </row>
@@ -46410,28 +46405,28 @@
       <c r="A76" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="B76" s="134" t="s">
+      <c r="B76" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C76" s="134" t="s">
+      <c r="C76" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="D76" s="134">
+      <c r="D76" s="130">
         <v>2</v>
       </c>
-      <c r="E76" s="134">
+      <c r="E76" s="130">
         <v>11</v>
       </c>
-      <c r="F76" s="134">
+      <c r="F76" s="130">
         <v>22</v>
       </c>
-      <c r="G76" s="134">
+      <c r="G76" s="130">
         <v>2</v>
       </c>
-      <c r="H76" s="134">
+      <c r="H76" s="130">
         <v>11</v>
       </c>
-      <c r="I76" s="134">
+      <c r="I76" s="130">
         <v>22</v>
       </c>
     </row>
@@ -46451,16 +46446,16 @@
       <c r="E77" s="14">
         <v>12</v>
       </c>
-      <c r="F77" s="130">
+      <c r="F77" s="14">
         <v>23</v>
       </c>
-      <c r="G77" s="130">
+      <c r="G77" s="14">
         <v>3</v>
       </c>
-      <c r="H77" s="130">
+      <c r="H77" s="14">
         <v>12</v>
       </c>
-      <c r="I77" s="130">
+      <c r="I77" s="14">
         <v>23</v>
       </c>
     </row>
@@ -46784,94 +46779,94 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="136" t="s">
+      <c r="A89" s="131" t="s">
         <v>199</v>
       </c>
-      <c r="B89" s="134" t="s">
+      <c r="B89" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C89" s="134" t="s">
+      <c r="C89" s="130" t="s">
         <v>57</v>
       </c>
-      <c r="D89" s="134">
+      <c r="D89" s="130">
         <v>1</v>
       </c>
-      <c r="E89" s="134">
+      <c r="E89" s="130">
         <v>2</v>
       </c>
-      <c r="F89" s="134">
+      <c r="F89" s="130">
         <v>3</v>
       </c>
-      <c r="G89" s="134">
+      <c r="G89" s="130">
         <v>1</v>
       </c>
-      <c r="H89" s="134">
+      <c r="H89" s="130">
         <v>2</v>
       </c>
-      <c r="I89" s="134">
+      <c r="I89" s="130">
         <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="136" t="s">
+      <c r="A90" s="131" t="s">
         <v>199</v>
       </c>
-      <c r="B90" s="134" t="s">
+      <c r="B90" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C90" s="134" t="s">
+      <c r="C90" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="D90" s="134">
+      <c r="D90" s="130">
         <v>1</v>
       </c>
-      <c r="E90" s="134">
+      <c r="E90" s="130">
         <v>10</v>
       </c>
-      <c r="F90" s="134">
+      <c r="F90" s="130">
         <v>21</v>
       </c>
-      <c r="G90" s="134">
+      <c r="G90" s="130">
         <v>1</v>
       </c>
-      <c r="H90" s="134">
+      <c r="H90" s="130">
         <v>10</v>
       </c>
-      <c r="I90" s="134">
+      <c r="I90" s="130">
         <v>21</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="136" t="s">
+      <c r="A91" s="131" t="s">
         <v>199</v>
       </c>
-      <c r="B91" s="134" t="s">
+      <c r="B91" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C91" s="134" t="s">
+      <c r="C91" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="D91" s="134">
+      <c r="D91" s="130">
         <v>2</v>
       </c>
-      <c r="E91" s="134">
+      <c r="E91" s="130">
         <v>11</v>
       </c>
-      <c r="F91" s="134">
+      <c r="F91" s="130">
         <v>22</v>
       </c>
-      <c r="G91" s="134">
+      <c r="G91" s="130">
         <v>2</v>
       </c>
-      <c r="H91" s="134">
+      <c r="H91" s="130">
         <v>11</v>
       </c>
-      <c r="I91" s="134">
+      <c r="I91" s="130">
         <v>22</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="136" t="s">
+      <c r="A92" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B92" s="14" t="s">
@@ -46900,7 +46895,7 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="136" t="s">
+      <c r="A93" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B93" s="14" t="s">
@@ -46929,7 +46924,7 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="136" t="s">
+      <c r="A94" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B94" s="14" t="s">
@@ -46958,7 +46953,7 @@
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="136" t="s">
+      <c r="A95" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B95" s="14" t="s">
@@ -46987,7 +46982,7 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="136" t="s">
+      <c r="A96" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B96" s="14" t="s">
@@ -47016,7 +47011,7 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="136" t="s">
+      <c r="A97" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B97" s="14" t="s">
@@ -47045,7 +47040,7 @@
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="136" t="s">
+      <c r="A98" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B98" s="14" t="s">
@@ -47074,7 +47069,7 @@
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="136" t="s">
+      <c r="A99" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B99" s="14" t="s">
@@ -47103,7 +47098,7 @@
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="136" t="s">
+      <c r="A100" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B100" s="14" t="s">
@@ -47132,7 +47127,7 @@
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="136" t="s">
+      <c r="A101" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B101" s="129" t="s">
@@ -47161,7 +47156,7 @@
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="136" t="s">
+      <c r="A102" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B102" s="129" t="s">
@@ -47190,7 +47185,7 @@
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="136" t="s">
+      <c r="A103" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B103" s="129" t="s">
@@ -47219,7 +47214,7 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="136" t="s">
+      <c r="A104" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B104" s="129" t="s">
@@ -47248,7 +47243,7 @@
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="136" t="s">
+      <c r="A105" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B105" s="129" t="s">
@@ -47277,7 +47272,7 @@
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="136" t="s">
+      <c r="A106" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B106" s="129" t="s">
@@ -47306,7 +47301,7 @@
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="136" t="s">
+      <c r="A107" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B107" s="2" t="s">
@@ -47335,7 +47330,7 @@
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="136" t="s">
+      <c r="A108" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B108" s="6" t="s">
@@ -47364,7 +47359,7 @@
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="136" t="s">
+      <c r="A109" s="131" t="s">
         <v>199</v>
       </c>
       <c r="B109" s="6" t="s">
@@ -47384,28 +47379,28 @@
       <c r="A110" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B110" s="134" t="s">
+      <c r="B110" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C110" s="134" t="s">
+      <c r="C110" s="130" t="s">
         <v>57</v>
       </c>
-      <c r="D110" s="134">
+      <c r="D110" s="130">
         <v>1</v>
       </c>
-      <c r="E110" s="134">
+      <c r="E110" s="130">
         <v>2</v>
       </c>
-      <c r="F110" s="134">
+      <c r="F110" s="130">
         <v>3</v>
       </c>
-      <c r="G110" s="134">
+      <c r="G110" s="130">
         <v>1</v>
       </c>
-      <c r="H110" s="134">
+      <c r="H110" s="130">
         <v>2</v>
       </c>
-      <c r="I110" s="134">
+      <c r="I110" s="130">
         <v>3</v>
       </c>
     </row>
@@ -47413,28 +47408,28 @@
       <c r="A111" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B111" s="134" t="s">
+      <c r="B111" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C111" s="134" t="s">
+      <c r="C111" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="D111" s="134">
+      <c r="D111" s="130">
         <v>1</v>
       </c>
-      <c r="E111" s="134">
+      <c r="E111" s="130">
         <v>10</v>
       </c>
-      <c r="F111" s="134">
+      <c r="F111" s="130">
         <v>21</v>
       </c>
-      <c r="G111" s="134">
+      <c r="G111" s="130">
         <v>1</v>
       </c>
-      <c r="H111" s="134">
+      <c r="H111" s="130">
         <v>10</v>
       </c>
-      <c r="I111" s="134">
+      <c r="I111" s="130">
         <v>21</v>
       </c>
     </row>
@@ -47442,28 +47437,28 @@
       <c r="A112" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B112" s="134" t="s">
+      <c r="B112" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C112" s="134" t="s">
+      <c r="C112" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="D112" s="134">
+      <c r="D112" s="130">
         <v>2</v>
       </c>
-      <c r="E112" s="134">
+      <c r="E112" s="130">
         <v>11</v>
       </c>
-      <c r="F112" s="134">
+      <c r="F112" s="130">
         <v>22</v>
       </c>
-      <c r="G112" s="134">
+      <c r="G112" s="130">
         <v>2</v>
       </c>
-      <c r="H112" s="134">
+      <c r="H112" s="130">
         <v>11</v>
       </c>
-      <c r="I112" s="134">
+      <c r="I112" s="130">
         <v>22</v>
       </c>
     </row>
@@ -47819,28 +47814,28 @@
       <c r="A125" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B125" s="134" t="s">
+      <c r="B125" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C125" s="134" t="s">
+      <c r="C125" s="130" t="s">
         <v>57</v>
       </c>
-      <c r="D125" s="134">
+      <c r="D125" s="130">
         <v>1</v>
       </c>
-      <c r="E125" s="134">
+      <c r="E125" s="130">
         <v>2</v>
       </c>
-      <c r="F125" s="134">
+      <c r="F125" s="130">
         <v>3</v>
       </c>
-      <c r="G125" s="134">
+      <c r="G125" s="130">
         <v>1</v>
       </c>
-      <c r="H125" s="134">
+      <c r="H125" s="130">
         <v>2</v>
       </c>
-      <c r="I125" s="134">
+      <c r="I125" s="130">
         <v>3</v>
       </c>
     </row>
@@ -47848,28 +47843,28 @@
       <c r="A126" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B126" s="134" t="s">
+      <c r="B126" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C126" s="134" t="s">
+      <c r="C126" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="D126" s="134">
+      <c r="D126" s="130">
         <v>1</v>
       </c>
-      <c r="E126" s="134">
+      <c r="E126" s="130">
         <v>10</v>
       </c>
-      <c r="F126" s="134">
+      <c r="F126" s="130">
         <v>21</v>
       </c>
-      <c r="G126" s="134">
+      <c r="G126" s="130">
         <v>1</v>
       </c>
-      <c r="H126" s="134">
+      <c r="H126" s="130">
         <v>10</v>
       </c>
-      <c r="I126" s="134">
+      <c r="I126" s="130">
         <v>21</v>
       </c>
     </row>
@@ -47877,28 +47872,28 @@
       <c r="A127" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B127" s="134" t="s">
+      <c r="B127" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C127" s="134" t="s">
+      <c r="C127" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="D127" s="134">
+      <c r="D127" s="130">
         <v>2</v>
       </c>
-      <c r="E127" s="137">
+      <c r="E127" s="130">
         <v>11</v>
       </c>
-      <c r="F127" s="137">
+      <c r="F127" s="130">
         <v>22</v>
       </c>
-      <c r="G127" s="137">
+      <c r="G127" s="130">
         <v>2</v>
       </c>
-      <c r="H127" s="137">
+      <c r="H127" s="130">
         <v>11</v>
       </c>
-      <c r="I127" s="137">
+      <c r="I127" s="130">
         <v>22</v>
       </c>
     </row>
@@ -48413,58 +48408,58 @@
       <c r="I145" s="6"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A146" s="138" t="s">
+      <c r="A146" s="132" t="s">
         <v>202</v>
       </c>
-      <c r="B146" s="134" t="s">
+      <c r="B146" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C146" s="134" t="s">
+      <c r="C146" s="130" t="s">
         <v>57</v>
       </c>
-      <c r="D146" s="134"/>
-      <c r="E146" s="134"/>
-      <c r="F146" s="134"/>
-      <c r="G146" s="134"/>
-      <c r="H146" s="134"/>
-      <c r="I146" s="134"/>
+      <c r="D146" s="130"/>
+      <c r="E146" s="130"/>
+      <c r="F146" s="130"/>
+      <c r="G146" s="130"/>
+      <c r="H146" s="130"/>
+      <c r="I146" s="130"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A147" s="138" t="s">
+      <c r="A147" s="132" t="s">
         <v>202</v>
       </c>
-      <c r="B147" s="134" t="s">
+      <c r="B147" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C147" s="134" t="s">
+      <c r="C147" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="D147" s="134"/>
-      <c r="E147" s="134"/>
-      <c r="F147" s="134"/>
-      <c r="G147" s="134"/>
-      <c r="H147" s="134"/>
-      <c r="I147" s="134"/>
+      <c r="D147" s="130"/>
+      <c r="E147" s="130"/>
+      <c r="F147" s="130"/>
+      <c r="G147" s="130"/>
+      <c r="H147" s="130"/>
+      <c r="I147" s="130"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A148" s="138" t="s">
+      <c r="A148" s="132" t="s">
         <v>202</v>
       </c>
-      <c r="B148" s="134" t="s">
+      <c r="B148" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C148" s="134" t="s">
+      <c r="C148" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="D148" s="134"/>
-      <c r="E148" s="134"/>
-      <c r="F148" s="134"/>
-      <c r="G148" s="134"/>
-      <c r="H148" s="134"/>
-      <c r="I148" s="134"/>
+      <c r="D148" s="130"/>
+      <c r="E148" s="130"/>
+      <c r="F148" s="130"/>
+      <c r="G148" s="130"/>
+      <c r="H148" s="130"/>
+      <c r="I148" s="130"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A149" s="138" t="s">
+      <c r="A149" s="132" t="s">
         <v>202</v>
       </c>
       <c r="B149" s="14" t="s">
@@ -48481,7 +48476,7 @@
       <c r="I149" s="14"/>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A150" s="138" t="s">
+      <c r="A150" s="132" t="s">
         <v>202</v>
       </c>
       <c r="B150" s="14" t="s">
@@ -48498,7 +48493,7 @@
       <c r="I150" s="14"/>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A151" s="138" t="s">
+      <c r="A151" s="132" t="s">
         <v>202</v>
       </c>
       <c r="B151" s="14" t="s">
@@ -48515,7 +48510,7 @@
       <c r="I151" s="14"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A152" s="138" t="s">
+      <c r="A152" s="132" t="s">
         <v>202</v>
       </c>
       <c r="B152" s="14" t="s">
@@ -48532,7 +48527,7 @@
       <c r="I152" s="14"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A153" s="138" t="s">
+      <c r="A153" s="132" t="s">
         <v>202</v>
       </c>
       <c r="B153" s="14" t="s">
@@ -48549,7 +48544,7 @@
       <c r="I153" s="14"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A154" s="138" t="s">
+      <c r="A154" s="132" t="s">
         <v>202</v>
       </c>
       <c r="B154" s="14" t="s">
@@ -48566,7 +48561,7 @@
       <c r="I154" s="14"/>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A155" s="138" t="s">
+      <c r="A155" s="132" t="s">
         <v>202</v>
       </c>
       <c r="B155" s="14" t="s">
@@ -48583,7 +48578,7 @@
       <c r="I155" s="14"/>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A156" s="138" t="s">
+      <c r="A156" s="132" t="s">
         <v>202</v>
       </c>
       <c r="B156" s="14" t="s">
@@ -48600,7 +48595,7 @@
       <c r="I156" s="14"/>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A157" s="138" t="s">
+      <c r="A157" s="132" t="s">
         <v>202</v>
       </c>
       <c r="B157" s="14" t="s">
@@ -48617,7 +48612,7 @@
       <c r="I157" s="14"/>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A158" s="138" t="s">
+      <c r="A158" s="132" t="s">
         <v>202</v>
       </c>
       <c r="B158" s="2" t="s">

</xml_diff>

<commit_message>
add slider scenarios and display missing slider options on report
</commit_message>
<xml_diff>
--- a/MMAPlus_Merchandising/MMAPlus_Merchandising.xlsx
+++ b/MMAPlus_Merchandising/MMAPlus_Merchandising.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9E4903-08C8-4B7E-827F-16F8AAE16F46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92DA1BE-4052-408D-ADA2-DF97B79678EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -683,9 +683,6 @@
     <t>Abnormal Shops</t>
   </si>
   <si>
-    <t>Merchandiser Score</t>
-  </si>
-  <si>
     <t>Info</t>
   </si>
   <si>
@@ -693,6 +690,9 @@
   </si>
   <si>
     <t>Logout</t>
+  </si>
+  <si>
+    <t>Merchandiser Scores</t>
   </si>
 </sst>
 </file>
@@ -55311,12 +55311,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -55371,22 +55371,22 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>